<commit_message>
feat: check boxes now working and can read the excell file
</commit_message>
<xml_diff>
--- a/commData.xlsx
+++ b/commData.xlsx
@@ -473,32 +473,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DummyName</t>
+          <t>Abangan Norte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>14.7661</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>120.9342</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>11417</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10080</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>6431</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -510,32 +510,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Abangan</t>
+          <t>Abangan Sur</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>14.7653</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>120.9437</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>10595</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>9750</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>6525</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -543,32 +543,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hotdog</t>
+          <t>Ibayo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>14.7535</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>120.9533</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>8310</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>

</xml_diff>